<commit_message>
added alignment scores (high and low) to RQ8
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ8.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ8.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96335B4B-4930-4568-B522-1BF4DD575E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01019E17-F117-430D-93CA-97B206371BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="101">
   <si>
     <t>Variables</t>
   </si>
@@ -51,7 +51,10 @@
     <t>Delegator KDMA</t>
   </si>
   <si>
-    <t>Alignment score (Participant|selected target)</t>
+    <t>Alignment score (Participant|high target)</t>
+  </si>
+  <si>
+    <t>Alignment score (Participant|low target)</t>
   </si>
   <si>
     <t>Assess_patient</t>
@@ -255,7 +258,10 @@
     <t>KDMA measurement from text scenario (ADEPT only)</t>
   </si>
   <si>
-    <t>Calculated alignment score between the KDMA measurement of a participant and a selected target</t>
+    <t>Calculated alignment score between the KDMA measurement of a participant and a high target (1.0 for ADEPT, qol-synth-HighExtreme, or vol-synth-HighExtreme)</t>
+  </si>
+  <si>
+    <t>Calculated alignment score between the KDMA measurement of a participant and a low target (0.0 for ADEPT, qol-synth-LowExtreme, or vol-synth-LowExtreme)</t>
   </si>
   <si>
     <t># of assessment actions taken per patient</t>
@@ -685,19 +691,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL4"/>
+  <dimension ref="A1:BM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="11" width="16.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="12" width="16.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="45.75">
+    <row r="1" spans="1:65" ht="45.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -890,557 +896,569 @@
       <c r="BL1" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:64" ht="30.75">
+    <row r="2" spans="1:65" ht="30.75">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AX2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BA2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:64" ht="106.5">
+    <row r="3" spans="1:65" ht="183">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="U3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AI3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AO3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AY3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AU3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BB3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="BC3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AZ3" s="1" t="s">
+      <c r="BE3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BA3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BD3" s="1" t="s">
+      <c r="BF3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BH3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BE3" s="1" t="s">
+      <c r="BI3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BF3" s="1" t="s">
+      <c r="BK3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BG3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="BH3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BJ3" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="BK3" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="BL3" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:64" ht="91.5">
+    <row r="4" spans="1:65" ht="91.5">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>96</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="AA4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AB4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AC4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="AG4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AH4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AI4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="AM4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AN4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AO4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="AS4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AT4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AU4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AV4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="AY4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AZ4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BB4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BC4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BD4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BA4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BB4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BC4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BD4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="BE4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BF4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BG4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BH4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BI4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BJ4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BG4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BH4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BI4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BJ4" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="BK4" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BL4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="BM4" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated variable definitions rq8
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ8.xlsx
+++ b/dashboard-ui/src/components/DRE-Research/variables/Variable Definitions RQ8.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01019E17-F117-430D-93CA-97B206371BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36AEEDC6-C58F-4AED-AA1F-927047584C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <t>Scenario</t>
   </si>
   <si>
-    <t>Delegator KDMA</t>
+    <t>Participant KDMA</t>
   </si>
   <si>
     <t>Alignment score (Participant|high target)</t>
@@ -694,7 +694,7 @@
   <dimension ref="A1:BM4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>